<commit_message>
Fixed issue with missing attachments
</commit_message>
<xml_diff>
--- a/.config/config.xlsx
+++ b/.config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GM00061060\UiPath\BlacklineItemWorking\.config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8DF630-303F-43CB-8332-AE17580BE9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E36018-17F4-4EAD-9D34-318285DE666F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3F103952-EB05-452A-A44A-30CC27982BEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F103952-EB05-452A-A44A-30CC27982BEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>AttachmentsMapTable</t>
   </si>
   <si>
-    <t>C:\Users\GM00061060\OneDrive - ICU Medical Inc\Process Automation - BlackLine\</t>
+    <t>C:\Users\GM00061060\OneDrive - ICU Medical Inc\Blackline Reconciliations - 2023\</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +577,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6b78b3fc-f09d-4cba-84d6-422834d4c347">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8ec9baa3-afa4-4ac0-b584-a71bf9c0ed20" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C71C7B27815D3449A08106381C0287D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b0d188d8626fa7870642b4e4b911241">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b78b3fc-f09d-4cba-84d6-422834d4c347" xmlns:ns3="8ec9baa3-afa4-4ac0-b584-a71bf9c0ed20" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f3aa84e18711634fa823cce7d22f212" ns2:_="" ns3:_="">
     <xsd:import namespace="6b78b3fc-f09d-4cba-84d6-422834d4c347"/>
@@ -777,27 +797,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6b78b3fc-f09d-4cba-84d6-422834d4c347">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8ec9baa3-afa4-4ac0-b584-a71bf9c0ed20" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8515B978-ED61-4AA7-855F-49F9C37C603F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6b78b3fc-f09d-4cba-84d6-422834d4c347"/>
+    <ds:schemaRef ds:uri="8ec9baa3-afa4-4ac0-b584-a71bf9c0ed20"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35ECBC2-4AFD-4777-8366-1213CE1A5536}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E42487B-207E-4983-B848-9163256C5372}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -814,23 +833,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8515B978-ED61-4AA7-855F-49F9C37C603F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6b78b3fc-f09d-4cba-84d6-422834d4c347"/>
-    <ds:schemaRef ds:uri="8ec9baa3-afa4-4ac0-b584-a71bf9c0ed20"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35ECBC2-4AFD-4777-8366-1213CE1A5536}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>